<commit_message>
bts and wnd files, dbg for Rosco, 8 seeds per wind speed
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ChineseOpenFastTutorial\AMPoWS\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309A675A-E795-4B83-AF23-ACA9BDF7C906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1815EC4B-F882-448D-860D-3CF4FD15111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="110">
   <si>
     <t>Location</t>
   </si>
@@ -321,6 +321,42 @@
   </si>
   <si>
     <t>./OutListParameters.xlsx</t>
+  </si>
+  <si>
+    <t>[401:1:408]</t>
+  </si>
+  <si>
+    <t>[601:1:608]</t>
+  </si>
+  <si>
+    <t>[801:1:808]</t>
+  </si>
+  <si>
+    <t>[1001:1:1008]</t>
+  </si>
+  <si>
+    <t>[1201:1:1208]</t>
+  </si>
+  <si>
+    <t>[1401:1:1408]</t>
+  </si>
+  <si>
+    <t>[1601:1:1608]</t>
+  </si>
+  <si>
+    <t>[1801:1:1808]</t>
+  </si>
+  <si>
+    <t>[2001:1:2008]</t>
+  </si>
+  <si>
+    <t>[2201:1:2208]</t>
+  </si>
+  <si>
+    <t>[2401:1:2408]</t>
+  </si>
+  <si>
+    <t>512</t>
   </si>
 </sst>
 </file>
@@ -797,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -946,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="14.25"/>
@@ -1036,10 +1072,10 @@
         <v>45</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1059,10 +1095,10 @@
         <v>45</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1082,10 +1118,10 @@
         <v>45</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1105,10 +1141,10 @@
         <v>45</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1128,10 +1164,10 @@
         <v>45</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1151,10 +1187,10 @@
         <v>45</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1174,10 +1210,10 @@
         <v>45</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1197,10 +1233,10 @@
         <v>45</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1220,10 +1256,10 @@
         <v>45</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1243,10 +1279,10 @@
         <v>45</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1266,10 +1302,10 @@
         <v>45</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new DLC 50 seeds xlsx
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ChineseOpenFastTutorial\AMPoWS\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1815EC4B-F882-448D-860D-3CF4FD15111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B201741B-3D7A-477E-91AF-817CA3C1BEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="109">
   <si>
     <t>Location</t>
   </si>
@@ -323,40 +323,37 @@
     <t>./OutListParameters.xlsx</t>
   </si>
   <si>
-    <t>[401:1:408]</t>
-  </si>
-  <si>
-    <t>[601:1:608]</t>
-  </si>
-  <si>
-    <t>[801:1:808]</t>
-  </si>
-  <si>
-    <t>[1001:1:1008]</t>
-  </si>
-  <si>
-    <t>[1201:1:1208]</t>
-  </si>
-  <si>
-    <t>[1401:1:1408]</t>
-  </si>
-  <si>
-    <t>[1601:1:1608]</t>
-  </si>
-  <si>
-    <t>[1801:1:1808]</t>
-  </si>
-  <si>
-    <t>[2001:1:2008]</t>
-  </si>
-  <si>
-    <t>[2201:1:2208]</t>
-  </si>
-  <si>
-    <t>[2401:1:2408]</t>
-  </si>
-  <si>
-    <t>512</t>
+    <t>[401:1:450]</t>
+  </si>
+  <si>
+    <t>[601:1:650]</t>
+  </si>
+  <si>
+    <t>[801:1:850]</t>
+  </si>
+  <si>
+    <t>[1001:1:1050]</t>
+  </si>
+  <si>
+    <t>[1201:1:1250]</t>
+  </si>
+  <si>
+    <t>[1401:1:1450]</t>
+  </si>
+  <si>
+    <t>[1601:1:1650]</t>
+  </si>
+  <si>
+    <t>[1801:1:1850]</t>
+  </si>
+  <si>
+    <t>[2001:1:2050]</t>
+  </si>
+  <si>
+    <t>[2201:1:2250]</t>
+  </si>
+  <si>
+    <t>[2401:1:2450]</t>
   </si>
 </sst>
 </file>
@@ -983,7 +980,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="14.25"/>
@@ -1072,7 +1069,7 @@
         <v>45</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>98</v>
@@ -1095,7 +1092,7 @@
         <v>45</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>99</v>
@@ -1118,7 +1115,7 @@
         <v>45</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>100</v>
@@ -1141,7 +1138,7 @@
         <v>45</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>101</v>
@@ -1164,7 +1161,7 @@
         <v>45</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>102</v>
@@ -1187,7 +1184,7 @@
         <v>45</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>103</v>
@@ -1210,7 +1207,7 @@
         <v>45</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>104</v>
@@ -1233,7 +1230,7 @@
         <v>45</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>105</v>
@@ -1256,7 +1253,7 @@
         <v>45</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>106</v>
@@ -1279,7 +1276,7 @@
         <v>45</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>107</v>
@@ -1302,7 +1299,7 @@
         <v>45</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
DLC 99 seeds, 700 seconds, roscoOpenFast original
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ChineseOpenFastTutorial\AMPoWS\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B201741B-3D7A-477E-91AF-817CA3C1BEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD0B880-5B42-45E3-82B3-8AC1BF615812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="110">
   <si>
     <t>Location</t>
   </si>
@@ -323,37 +323,40 @@
     <t>./OutListParameters.xlsx</t>
   </si>
   <si>
-    <t>[401:1:450]</t>
-  </si>
-  <si>
-    <t>[601:1:650]</t>
-  </si>
-  <si>
-    <t>[801:1:850]</t>
-  </si>
-  <si>
-    <t>[1001:1:1050]</t>
-  </si>
-  <si>
-    <t>[1201:1:1250]</t>
-  </si>
-  <si>
-    <t>[1401:1:1450]</t>
-  </si>
-  <si>
-    <t>[1601:1:1650]</t>
-  </si>
-  <si>
-    <t>[1801:1:1850]</t>
-  </si>
-  <si>
-    <t>[2001:1:2050]</t>
-  </si>
-  <si>
-    <t>[2201:1:2250]</t>
-  </si>
-  <si>
-    <t>[2401:1:2450]</t>
+    <t>700</t>
+  </si>
+  <si>
+    <t>[401:1:499]</t>
+  </si>
+  <si>
+    <t>[601:1:699]</t>
+  </si>
+  <si>
+    <t>[801:1:899]</t>
+  </si>
+  <si>
+    <t>[1001:1:1099]</t>
+  </si>
+  <si>
+    <t>[1201:1:1299]</t>
+  </si>
+  <si>
+    <t>[1401:1:1499]</t>
+  </si>
+  <si>
+    <t>[1601:1:1699]</t>
+  </si>
+  <si>
+    <t>[1801:1:1899]</t>
+  </si>
+  <si>
+    <t>[2001:1:2099]</t>
+  </si>
+  <si>
+    <t>[2201:1:2299]</t>
+  </si>
+  <si>
+    <t>[2401:1:2499]</t>
   </si>
 </sst>
 </file>
@@ -831,7 +834,7 @@
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="14.25"/>
@@ -980,7 +983,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="14.25"/>
@@ -1069,10 +1072,10 @@
         <v>45</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1092,10 +1095,10 @@
         <v>45</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1115,10 +1118,10 @@
         <v>45</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1138,10 +1141,10 @@
         <v>45</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1161,10 +1164,10 @@
         <v>45</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1184,10 +1187,10 @@
         <v>45</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1207,10 +1210,10 @@
         <v>45</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1230,10 +1233,10 @@
         <v>45</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1253,10 +1256,10 @@
         <v>45</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1276,10 +1279,10 @@
         <v>45</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1299,10 +1302,10 @@
         <v>45</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1317,10 +1320,13 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="16" max="16" width="9.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="6" t="s">

</xml_diff>

<commit_message>
Before Meeting with David
</commit_message>
<xml_diff>
--- a/examples/openFAST_config.xlsx
+++ b/examples/openFAST_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25915"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ChineseOpenFastTutorial\AMPoWS\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{842DF77F-66AD-4C9D-B8A3-96577C2C0E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABB1A185-A433-44D8-8C2A-CD434A893B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,277 +197,277 @@
     <t>A</t>
   </si>
   <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>[401:1:499]</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>7.1821</t>
+  </si>
+  <si>
+    <t>0.052297</t>
+  </si>
+  <si>
+    <t>1p2_6</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>[601:1:699]</t>
+  </si>
+  <si>
+    <t>7.9391</t>
+  </si>
+  <si>
+    <t>0.11526</t>
+  </si>
+  <si>
+    <t>1p2_8</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>[801:1:899]</t>
+  </si>
+  <si>
+    <t>9.1431</t>
+  </si>
+  <si>
+    <t>0.19602</t>
+  </si>
+  <si>
+    <t>1p2_10</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>[1001:1:1099]</t>
+  </si>
+  <si>
+    <t>11.4289</t>
+  </si>
+  <si>
+    <t>0.31416</t>
+  </si>
+  <si>
+    <t>1p2_12</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>[1201:1:1299]</t>
+  </si>
+  <si>
+    <t>3.8283</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>0.31445</t>
+  </si>
+  <si>
+    <t>1p2_14</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>[1401:1:1499]</t>
+  </si>
+  <si>
+    <t>8.6723</t>
+  </si>
+  <si>
+    <t>0.24187</t>
+  </si>
+  <si>
+    <t>1p2_16</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>[1601:1:1699]</t>
+  </si>
+  <si>
+    <t>12.0574</t>
+  </si>
+  <si>
+    <t>0.20547</t>
+  </si>
+  <si>
+    <t>1p_18</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>[1801:1:1899]</t>
+  </si>
+  <si>
+    <t>14.921</t>
+  </si>
+  <si>
+    <t>0.18244</t>
+  </si>
+  <si>
+    <t>1p_20</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>[2001:1:2099]</t>
+  </si>
+  <si>
+    <t>17.4739</t>
+  </si>
+  <si>
+    <t>0.16693</t>
+  </si>
+  <si>
+    <t>1p_22</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>[2201:1:2299]</t>
+  </si>
+  <si>
+    <t>19.9422</t>
+  </si>
+  <si>
+    <t>0.1544</t>
+  </si>
+  <si>
+    <t>1p_24</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>[2401:1:2499]</t>
+  </si>
+  <si>
+    <t>22.3452</t>
+  </si>
+  <si>
+    <t>0.14482</t>
+  </si>
+  <si>
+    <t>1p1</t>
+  </si>
+  <si>
+    <t>[4:2:24]</t>
+  </si>
+  <si>
+    <t>1p3</t>
+  </si>
+  <si>
+    <t>ETM</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;[5 7]</t>
+  </si>
+  <si>
+    <t>1p4</t>
+  </si>
+  <si>
+    <t>IEC:ECD+R:ECD+R+2.0:ECD+R-2.0</t>
+  </si>
+  <si>
+    <t>1p5</t>
+  </si>
+  <si>
+    <t>IEC:EWSH+12.0</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>impulse</t>
+  </si>
+  <si>
+    <t>IMP:+1/5</t>
+  </si>
+  <si>
+    <t>[v_r-2 v_r v_r+2]</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>ramp</t>
+  </si>
+  <si>
+    <t>RMP:50</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>coh</t>
+  </si>
+  <si>
+    <t>BTS:NTM_URef-%d_turbsim_coh</t>
+  </si>
+  <si>
+    <t>[10 20]</t>
+  </si>
+  <si>
+    <t>1p2</t>
+  </si>
+  <si>
+    <t>[401:1:406]</t>
+  </si>
+  <si>
+    <t>[601:1:606]</t>
+  </si>
+  <si>
+    <t>[801:1:806]</t>
+  </si>
+  <si>
+    <t>[1001:1:1006]</t>
+  </si>
+  <si>
+    <t>[1201:1:1206]</t>
+  </si>
+  <si>
+    <t>[1401:1:1406]</t>
+  </si>
+  <si>
+    <t>[1601:1:1606]</t>
+  </si>
+  <si>
+    <t>[1801:1:1806]</t>
+  </si>
+  <si>
+    <t>[2001:1:2006]</t>
+  </si>
+  <si>
+    <t>[2201:1:2206]</t>
+  </si>
+  <si>
+    <t>[2401:1:2406]</t>
+  </si>
+  <si>
     <t>700</t>
-  </si>
-  <si>
-    <t>[401:1:499]</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>7.1821</t>
-  </si>
-  <si>
-    <t>0.052297</t>
-  </si>
-  <si>
-    <t>1p2_6</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>[601:1:699]</t>
-  </si>
-  <si>
-    <t>7.9391</t>
-  </si>
-  <si>
-    <t>0.11526</t>
-  </si>
-  <si>
-    <t>1p2_8</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>[801:1:899]</t>
-  </si>
-  <si>
-    <t>9.1431</t>
-  </si>
-  <si>
-    <t>0.19602</t>
-  </si>
-  <si>
-    <t>1p2_10</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>[1001:1:1099]</t>
-  </si>
-  <si>
-    <t>11.4289</t>
-  </si>
-  <si>
-    <t>0.31416</t>
-  </si>
-  <si>
-    <t>1p2_12</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>[1201:1:1299]</t>
-  </si>
-  <si>
-    <t>3.8283</t>
-  </si>
-  <si>
-    <t>12.1</t>
-  </si>
-  <si>
-    <t>0.31445</t>
-  </si>
-  <si>
-    <t>1p2_14</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>[1401:1:1499]</t>
-  </si>
-  <si>
-    <t>8.6723</t>
-  </si>
-  <si>
-    <t>0.24187</t>
-  </si>
-  <si>
-    <t>1p2_16</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>[1601:1:1699]</t>
-  </si>
-  <si>
-    <t>12.0574</t>
-  </si>
-  <si>
-    <t>0.20547</t>
-  </si>
-  <si>
-    <t>1p_18</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>[1801:1:1899]</t>
-  </si>
-  <si>
-    <t>14.921</t>
-  </si>
-  <si>
-    <t>0.18244</t>
-  </si>
-  <si>
-    <t>1p_20</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>[2001:1:2099]</t>
-  </si>
-  <si>
-    <t>17.4739</t>
-  </si>
-  <si>
-    <t>0.16693</t>
-  </si>
-  <si>
-    <t>1p_22</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>[2201:1:2299]</t>
-  </si>
-  <si>
-    <t>19.9422</t>
-  </si>
-  <si>
-    <t>0.1544</t>
-  </si>
-  <si>
-    <t>1p_24</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>[2401:1:2499]</t>
-  </si>
-  <si>
-    <t>22.3452</t>
-  </si>
-  <si>
-    <t>0.14482</t>
-  </si>
-  <si>
-    <t>1p1</t>
-  </si>
-  <si>
-    <t>[4:2:24]</t>
-  </si>
-  <si>
-    <t>1p3</t>
-  </si>
-  <si>
-    <t>ETM</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>&lt;b&gt;[5 7]</t>
-  </si>
-  <si>
-    <t>1p4</t>
-  </si>
-  <si>
-    <t>IEC:ECD+R:ECD+R+2.0:ECD+R-2.0</t>
-  </si>
-  <si>
-    <t>1p5</t>
-  </si>
-  <si>
-    <t>IEC:EWSH+12.0</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>impulse</t>
-  </si>
-  <si>
-    <t>IMP:+1/5</t>
-  </si>
-  <si>
-    <t>[v_r-2 v_r v_r+2]</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>ramp</t>
-  </si>
-  <si>
-    <t>RMP:50</t>
-  </si>
-  <si>
-    <t>1100</t>
-  </si>
-  <si>
-    <t>coh</t>
-  </si>
-  <si>
-    <t>BTS:NTM_URef-%d_turbsim_coh</t>
-  </si>
-  <si>
-    <t>[10 20]</t>
-  </si>
-  <si>
-    <t>1p2</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>[401:1:406]</t>
-  </si>
-  <si>
-    <t>[601:1:606]</t>
-  </si>
-  <si>
-    <t>[801:1:806]</t>
-  </si>
-  <si>
-    <t>[1001:1:1006]</t>
-  </si>
-  <si>
-    <t>[1201:1:1206]</t>
-  </si>
-  <si>
-    <t>[1401:1:1406]</t>
-  </si>
-  <si>
-    <t>[1601:1:1606]</t>
-  </si>
-  <si>
-    <t>[1801:1:1806]</t>
-  </si>
-  <si>
-    <t>[2001:1:2006]</t>
-  </si>
-  <si>
-    <t>[2201:1:2206]</t>
-  </si>
-  <si>
-    <t>[2401:1:2406]</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -570,7 +570,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,7 +1104,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H2" sqref="H2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="14.25"/>
@@ -1180,7 +1179,7 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1910,11 +1909,11 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1936,11 +1935,11 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1962,11 +1961,11 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1988,11 +1987,11 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2014,11 +2013,11 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2040,11 +2039,11 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2066,11 +2065,11 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2092,11 +2091,11 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2118,11 +2117,11 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2144,11 +2143,11 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2170,11 +2169,11 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="4" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2255,7 +2254,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4" t="s">
@@ -2291,7 +2290,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
@@ -2327,7 +2326,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
@@ -2357,7 +2356,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
@@ -2387,7 +2386,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
@@ -2417,7 +2416,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
@@ -2447,7 +2446,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
@@ -2477,7 +2476,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
@@ -2507,7 +2506,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
@@ -2537,7 +2536,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
@@ -2567,7 +2566,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="4" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">

</xml_diff>